<commit_message>
alg2 test correction #2
Former-commit-id: 56f39a5526c08c48ebf578eccae5ab2ae1b3c8f8
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_alg2.xlsx
+++ b/tests/test_data/test_dfs_alg2.xlsx
@@ -202,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -233,8 +233,10 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AQ3" sqref="AQ3"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,12 +798,12 @@
       </c>
       <c r="AH2" s="12">
         <f>AI2+AE2</f>
-        <v>834</v>
+        <v>650</v>
       </c>
       <c r="AI2" s="1">
-        <v>644</v>
-      </c>
-      <c r="AJ2" s="27">
+        <v>460</v>
+      </c>
+      <c r="AJ2" s="26">
         <f>$AP2-$AQ2</f>
         <v>400</v>
       </c>
@@ -817,7 +819,7 @@
         <v>800</v>
       </c>
       <c r="AN2" s="9"/>
-      <c r="AO2" s="12">
+      <c r="AO2" s="26">
         <f>AL2+AM2</f>
         <v>1765</v>
       </c>
@@ -941,10 +943,10 @@
       </c>
       <c r="AH3" s="12">
         <f t="shared" ref="AH3:AH13" si="6">AI3+AE3</f>
-        <v>834</v>
+        <v>650</v>
       </c>
       <c r="AI3" s="1">
-        <v>644</v>
+        <v>460</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="7">$AP3-$AQ3</f>
@@ -962,7 +964,7 @@
         <v>800</v>
       </c>
       <c r="AN3" s="9"/>
-      <c r="AO3" s="12">
+      <c r="AO3" s="26">
         <f t="shared" ref="AO3:AO16" si="9">AL3+AM3</f>
         <v>1765</v>
       </c>
@@ -1085,10 +1087,10 @@
       </c>
       <c r="AH4" s="12">
         <f t="shared" si="6"/>
-        <v>834</v>
+        <v>650</v>
       </c>
       <c r="AI4" s="1">
-        <v>644</v>
+        <v>460</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="7"/>
@@ -1106,7 +1108,7 @@
         <v>800</v>
       </c>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="12">
+      <c r="AO4" s="26">
         <f t="shared" si="9"/>
         <v>1765</v>
       </c>
@@ -1227,10 +1229,10 @@
       </c>
       <c r="AH5" s="23">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>400</v>
       </c>
       <c r="AI5" s="21">
-        <v>512</v>
+        <v>400</v>
       </c>
       <c r="AJ5" s="21">
         <f t="shared" si="7"/>
@@ -1248,7 +1250,7 @@
         <v>480</v>
       </c>
       <c r="AN5" s="9"/>
-      <c r="AO5" s="23">
+      <c r="AO5" s="27">
         <f t="shared" si="9"/>
         <v>1170</v>
       </c>
@@ -1373,10 +1375,10 @@
       </c>
       <c r="AH6" s="24">
         <f t="shared" si="6"/>
-        <v>512</v>
+        <v>400</v>
       </c>
       <c r="AI6" s="22">
-        <v>512</v>
+        <v>400</v>
       </c>
       <c r="AJ6" s="22">
         <f t="shared" si="7"/>
@@ -1394,7 +1396,7 @@
         <v>480</v>
       </c>
       <c r="AN6" s="9"/>
-      <c r="AO6" s="26">
+      <c r="AO6" s="28">
         <f t="shared" si="9"/>
         <v>1170</v>
       </c>
@@ -1518,10 +1520,10 @@
       </c>
       <c r="AH7" s="23">
         <f t="shared" si="6"/>
-        <v>719.6</v>
+        <v>578.5</v>
       </c>
       <c r="AI7" s="21">
-        <v>555.6</v>
+        <v>414.5</v>
       </c>
       <c r="AJ7" s="21">
         <f t="shared" si="7"/>
@@ -1540,7 +1542,7 @@
         <v>480</v>
       </c>
       <c r="AN7" s="9"/>
-      <c r="AO7" s="23">
+      <c r="AO7" s="27">
         <f t="shared" si="9"/>
         <v>1183.6399999999999</v>
       </c>
@@ -1665,10 +1667,10 @@
       </c>
       <c r="AH8" s="24">
         <f t="shared" si="6"/>
-        <v>719.6</v>
+        <v>578.5</v>
       </c>
       <c r="AI8" s="22">
-        <v>555.6</v>
+        <v>414.5</v>
       </c>
       <c r="AJ8" s="22">
         <f t="shared" si="7"/>
@@ -1687,7 +1689,7 @@
         <v>480</v>
       </c>
       <c r="AN8" s="9"/>
-      <c r="AO8" s="24">
+      <c r="AO8" s="29">
         <f t="shared" si="9"/>
         <v>1183.6399999999999</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>970</v>
       </c>
       <c r="AN9" s="10"/>
-      <c r="AO9" s="23">
+      <c r="AO9" s="27">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
@@ -1979,7 +1981,7 @@
         <v>970</v>
       </c>
       <c r="AN10" s="9"/>
-      <c r="AO10" s="24">
+      <c r="AO10" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
@@ -2125,7 +2127,7 @@
         <v>970</v>
       </c>
       <c r="AN11" s="9"/>
-      <c r="AO11" s="24">
+      <c r="AO11" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
@@ -2270,7 +2272,7 @@
         <v>970</v>
       </c>
       <c r="AN12" s="9"/>
-      <c r="AO12" s="24">
+      <c r="AO12" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
@@ -2415,7 +2417,7 @@
         <v>970</v>
       </c>
       <c r="AN13" s="9"/>
-      <c r="AO13" s="24">
+      <c r="AO13" s="29">
         <f t="shared" si="9"/>
         <v>2281</v>
       </c>
@@ -2558,7 +2560,7 @@
         <v>830</v>
       </c>
       <c r="AN14" s="2"/>
-      <c r="AO14" s="23">
+      <c r="AO14" s="27">
         <f t="shared" si="9"/>
         <v>1703</v>
       </c>
@@ -2676,10 +2678,10 @@
       </c>
       <c r="AH15" s="1">
         <f>AI15+AE15</f>
-        <v>1578.1</v>
+        <v>1289</v>
       </c>
       <c r="AI15" s="1">
-        <v>1578.1</v>
+        <v>1289</v>
       </c>
       <c r="AJ15" s="1">
         <f t="shared" si="7"/>
@@ -2696,7 +2698,7 @@
         <f t="shared" ref="AM15:AM16" si="15">I15+J15</f>
         <v>830</v>
       </c>
-      <c r="AO15" s="12">
+      <c r="AO15" s="26">
         <f t="shared" si="9"/>
         <v>1703</v>
       </c>
@@ -2813,10 +2815,10 @@
       </c>
       <c r="AH16" s="1">
         <f t="shared" si="13"/>
-        <v>1578.1</v>
-      </c>
-      <c r="AI16" s="22">
-        <v>1578.1</v>
+        <v>1289</v>
+      </c>
+      <c r="AI16" s="1">
+        <v>1289</v>
       </c>
       <c r="AJ16" s="1">
         <f t="shared" si="7"/>
@@ -2833,7 +2835,7 @@
         <f t="shared" si="15"/>
         <v>830</v>
       </c>
-      <c r="AO16" s="12">
+      <c r="AO16" s="26">
         <f t="shared" si="9"/>
         <v>1703</v>
       </c>

</xml_diff>

<commit_message>
alg2 test correction #3
Former-commit-id: c83137c1af8ebf15f454da2b331b3314cc10cebd
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_alg2.xlsx
+++ b/tests/test_data/test_dfs_alg2.xlsx
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AO7" sqref="AO7"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,14 +1229,14 @@
       </c>
       <c r="AH5" s="23">
         <f t="shared" si="6"/>
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="AI5" s="21">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="AJ5" s="21">
         <f t="shared" si="7"/>
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="AK5" s="2">
         <v>0</v>
@@ -1255,8 +1255,8 @@
         <v>1170</v>
       </c>
       <c r="AP5" s="15">
-        <f t="shared" ref="AP5:AP16" si="10">U5-AB5-AC5-AD5</f>
-        <v>640</v>
+        <f>U5+Y5-AB5-AC5-AD5</f>
+        <v>740</v>
       </c>
       <c r="AQ5">
         <f>100+0.2*(U5-100)</f>
@@ -1375,10 +1375,10 @@
       </c>
       <c r="AH6" s="24">
         <f t="shared" si="6"/>
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="AI6" s="22">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="AJ6" s="22">
         <f t="shared" si="7"/>
@@ -1401,7 +1401,7 @@
         <v>1170</v>
       </c>
       <c r="AP6" s="19">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="AP5:AP16" si="10">U6-AB6-AC6-AD6</f>
         <v>0</v>
       </c>
       <c r="AQ6" s="6">
@@ -1519,15 +1519,15 @@
         <v>2009</v>
       </c>
       <c r="AH7" s="23">
-        <f t="shared" si="6"/>
-        <v>578.5</v>
+        <f>AI7+AE7</f>
+        <v>848.5</v>
       </c>
       <c r="AI7" s="21">
-        <v>414.5</v>
+        <v>684.5</v>
       </c>
       <c r="AJ7" s="21">
         <f t="shared" si="7"/>
-        <v>414.5</v>
+        <v>684.5</v>
       </c>
       <c r="AK7" s="2">
         <f>MAX(0.12*P7,0.36)</f>
@@ -1547,12 +1547,12 @@
         <v>1183.6399999999999</v>
       </c>
       <c r="AP7" s="15">
-        <f t="shared" si="10"/>
-        <v>694.5</v>
+        <f>U7+Y7-AB7-AC7-AD7</f>
+        <v>944.5</v>
       </c>
       <c r="AQ7">
-        <f>100+0.2*(U7-100)</f>
-        <v>280</v>
+        <f>100+0.2*(700)+0.1*200</f>
+        <v>260</v>
       </c>
       <c r="AR7" s="10"/>
       <c r="AS7" s="8"/>
@@ -1667,10 +1667,10 @@
       </c>
       <c r="AH8" s="24">
         <f t="shared" si="6"/>
-        <v>578.5</v>
+        <v>848.5</v>
       </c>
       <c r="AI8" s="22">
-        <v>414.5</v>
+        <v>684.5</v>
       </c>
       <c r="AJ8" s="22">
         <f t="shared" si="7"/>

</xml_diff>

<commit_message>
ALG2 is now more restrictive in housing costs
Former-commit-id: a6508a23b1cbb812016a2be2c8669c494936a1c6
Former-commit-id: 38476d83843995084e610430234ba2d3eb234e1d
</commit_message>
<xml_diff>
--- a/tests/test_data/test_dfs_alg2.xlsx
+++ b/tests/test_data/test_dfs_alg2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>hid</t>
   </si>
@@ -149,6 +149,18 @@
   </si>
   <si>
     <t>uhv</t>
+  </si>
+  <si>
+    <t>wohnfl</t>
+  </si>
+  <si>
+    <t>eigentum</t>
+  </si>
+  <si>
+    <t>cost_per_sqm</t>
+  </si>
+  <si>
+    <t>wohnfl_just</t>
   </si>
 </sst>
 </file>
@@ -550,23 +562,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV29"/>
+  <dimension ref="A1:AX29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AI17" sqref="AI17"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AN28" sqref="AN28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="15" width="9.140625" customWidth="1"/>
-    <col min="35" max="35" width="15.7109375" customWidth="1"/>
-    <col min="39" max="39" width="12.5703125" customWidth="1"/>
-    <col min="40" max="40" width="14.7109375" customWidth="1"/>
-    <col min="41" max="41" width="16.140625" customWidth="1"/>
-    <col min="42" max="42" width="9.28515625" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" customWidth="1"/>
+    <col min="37" max="37" width="15.7109375" customWidth="1"/>
+    <col min="41" max="41" width="12.5703125" customWidth="1"/>
+    <col min="42" max="42" width="14.7109375" customWidth="1"/>
+    <col min="43" max="43" width="16.140625" customWidth="1"/>
+    <col min="44" max="44" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -598,112 +610,124 @@
         <v>12</v>
       </c>
       <c r="K1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AE1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AF1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AG1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="13" t="s">
+      <c r="AH1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="13" t="s">
+      <c r="AI1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AJ1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AL1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AM1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AN1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AO1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AP1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="14" t="s">
+      <c r="AQ1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AR1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AS1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="13" t="s">
+      <c r="AT1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="13" t="s">
+      <c r="AU1" s="13" t="s">
         <v>43</v>
       </c>
+      <c r="AV1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="13" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -727,7 +751,7 @@
         <v>30</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H18" si="0">AH2-G2</f>
+        <f t="shared" ref="H2:H18" si="0">AJ2-G2</f>
         <v>1986</v>
       </c>
       <c r="I2">
@@ -736,47 +760,47 @@
       <c r="J2">
         <v>100</v>
       </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <f>E2-P2</f>
-        <v>2</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
+      <c r="K2">
+        <v>75</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <f>E2-R2</f>
+        <v>2</v>
       </c>
       <c r="O2">
-        <f>P2</f>
         <v>1</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2" s="2">
-        <v>0</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0</v>
-      </c>
-      <c r="S2" s="3">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
+      <c r="Q2">
+        <f>R2</f>
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
         <v>1000</v>
       </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
       <c r="X2">
         <v>0</v>
       </c>
@@ -790,67 +814,81 @@
         <v>0</v>
       </c>
       <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
         <v>100</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>20</v>
       </c>
-      <c r="AD2">
-        <f t="shared" ref="AD2:AD15" si="1">0.2*U2</f>
+      <c r="AF2">
+        <f t="shared" ref="AF2:AF15" si="1">0.2*W2</f>
         <v>200</v>
       </c>
-      <c r="AE2">
-        <f>P2*190</f>
+      <c r="AG2">
+        <f>R2*190</f>
         <v>190</v>
       </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
       <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
         <v>2016</v>
       </c>
-      <c r="AI2" s="12">
-        <f>AJ2+AE2</f>
+      <c r="AK2" s="12">
+        <f>AL2+AG2</f>
         <v>650</v>
       </c>
-      <c r="AJ2" s="1">
+      <c r="AL2" s="1">
         <v>460</v>
       </c>
-      <c r="AK2" s="26">
-        <f>$AP2-$AQ2</f>
+      <c r="AM2" s="26">
+        <f t="shared" ref="AM2:AM21" si="2">$AR2-$AS2</f>
         <v>400</v>
       </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
-      <c r="AM2">
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
         <f>2*364+237</f>
         <v>965</v>
       </c>
-      <c r="AN2" s="9">
-        <f t="shared" ref="AN2:AN14" si="2">I2+J2</f>
-        <v>800</v>
-      </c>
-      <c r="AO2" s="26">
-        <f>AM2+AN2</f>
-        <v>1765</v>
-      </c>
-      <c r="AP2" s="11">
-        <f>U2-AB2-AC2-AD2</f>
+      <c r="AP2" s="9">
+        <f>AV2*AW2</f>
+        <v>750</v>
+      </c>
+      <c r="AQ2" s="26">
+        <f>AO2+AP2</f>
+        <v>1715</v>
+      </c>
+      <c r="AR2" s="11">
+        <f>W2-AD2-AE2-AF2</f>
         <v>680</v>
       </c>
-      <c r="AQ2">
-        <f>100+0.2*(U2-100)</f>
+      <c r="AS2">
+        <f>100+0.2*(W2-100)</f>
         <v>280</v>
       </c>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="5"/>
-      <c r="AV2" s="11"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2">
+        <f>MIN(10,(I2+J2)/K2)</f>
+        <v>10</v>
+      </c>
+      <c r="AW2">
+        <f>MIN(45+(E2-1)*15,K2)</f>
+        <v>75</v>
+      </c>
+      <c r="AX2" s="11"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -882,43 +920,43 @@
       <c r="J3">
         <v>100</v>
       </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L13" si="3">E3-P3</f>
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
+      <c r="K3">
+        <v>75</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <f t="shared" ref="N3:N13" si="3">E3-R3</f>
+        <v>2</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O13" si="4">P3</f>
         <v>1</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
-      <c r="Q3" s="3">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3">
-        <v>0</v>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q13" si="4">R3</f>
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
       </c>
       <c r="S3" s="3">
         <v>0</v>
       </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3">
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
         <v>0</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -939,64 +977,78 @@
         <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" ref="AC3:AC14" si="5">0.055*AB3</f>
         <v>0</v>
       </c>
       <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE14" si="5">0.055*AD3</f>
+        <v>0</v>
+      </c>
+      <c r="AF3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE3">
-        <f>P3*190</f>
+      <c r="AG3">
+        <f>R3*190</f>
         <v>190</v>
       </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
       <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
         <v>2016</v>
       </c>
-      <c r="AI3" s="12">
-        <f t="shared" ref="AI3:AI13" si="6">AJ3+AE3</f>
+      <c r="AK3" s="12">
+        <f t="shared" ref="AK3:AK13" si="6">AL3+AG3</f>
         <v>650</v>
       </c>
-      <c r="AJ3" s="1">
+      <c r="AL3" s="1">
         <v>460</v>
       </c>
-      <c r="AK3" s="1">
-        <f t="shared" ref="AK3:AK21" si="7">$AP3-$AQ3</f>
-        <v>0</v>
-      </c>
-      <c r="AL3">
-        <v>0</v>
-      </c>
-      <c r="AM3">
-        <f t="shared" ref="AM3:AM4" si="8">2*364+237</f>
+      <c r="AM3" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" ref="AO3:AO4" si="7">2*364+237</f>
         <v>965</v>
       </c>
-      <c r="AN3" s="9">
-        <f t="shared" si="2"/>
-        <v>800</v>
-      </c>
-      <c r="AO3" s="26">
-        <f t="shared" ref="AO3:AO16" si="9">AM3+AN3</f>
-        <v>1765</v>
-      </c>
-      <c r="AP3" s="11">
-        <f>U3-AB3-AC3-AD3</f>
-        <v>0</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="9"/>
-      <c r="AS3" s="5"/>
-      <c r="AV3" s="11"/>
+      <c r="AP3" s="9">
+        <f t="shared" ref="AP3:AP21" si="8">AV3*AW3</f>
+        <v>750</v>
+      </c>
+      <c r="AQ3" s="26">
+        <f t="shared" ref="AQ3:AQ16" si="9">AO3+AP3</f>
+        <v>1715</v>
+      </c>
+      <c r="AR3" s="11">
+        <f>W3-AD3-AE3-AF3</f>
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="5"/>
+      <c r="AV3">
+        <f t="shared" ref="AV3:AV21" si="10">MIN(10,(I3+J3)/K3)</f>
+        <v>10</v>
+      </c>
+      <c r="AW3">
+        <f t="shared" ref="AW3:AW21" si="11">MIN(45+(E3-1)*15,K3)</f>
+        <v>75</v>
+      </c>
+      <c r="AX3" s="11"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1028,47 +1080,47 @@
       <c r="J4">
         <v>100</v>
       </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4">
+      <c r="K4">
+        <v>75</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
       <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
         <v>200</v>
       </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
       <c r="X4">
         <v>0</v>
       </c>
@@ -1085,63 +1137,77 @@
         <v>0</v>
       </c>
       <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="AE4">
-        <f>P4*190</f>
+      <c r="AG4">
+        <f>R4*190</f>
         <v>190</v>
       </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>0</v>
-      </c>
       <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
         <v>2016</v>
       </c>
-      <c r="AI4" s="12">
+      <c r="AK4" s="12">
         <f t="shared" si="6"/>
         <v>650</v>
       </c>
-      <c r="AJ4" s="1">
+      <c r="AL4" s="1">
         <v>460</v>
       </c>
-      <c r="AK4" s="1">
+      <c r="AM4" s="1">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
         <f t="shared" si="7"/>
-        <v>60</v>
-      </c>
-      <c r="AL4">
-        <v>0</v>
-      </c>
-      <c r="AM4">
+        <v>965</v>
+      </c>
+      <c r="AP4" s="9">
         <f t="shared" si="8"/>
-        <v>965</v>
-      </c>
-      <c r="AN4" s="9">
-        <f t="shared" si="2"/>
-        <v>800</v>
-      </c>
-      <c r="AO4" s="26">
+        <v>750</v>
+      </c>
+      <c r="AQ4" s="26">
         <f t="shared" si="9"/>
-        <v>1765</v>
-      </c>
-      <c r="AP4" s="11">
+        <v>1715</v>
+      </c>
+      <c r="AR4" s="11">
         <v>160</v>
       </c>
-      <c r="AQ4">
+      <c r="AS4">
         <v>100</v>
       </c>
-      <c r="AR4" s="9"/>
-      <c r="AS4" s="5"/>
-      <c r="AV4" s="11"/>
+      <c r="AT4" s="9"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="AW4">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="AX4" s="11"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -1173,29 +1239,29 @@
       <c r="J5" s="2">
         <v>80</v>
       </c>
-      <c r="K5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
+      <c r="K5" s="2">
+        <v>70</v>
+      </c>
+      <c r="L5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
       <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
       <c r="R5" s="2">
         <v>0</v>
       </c>
@@ -1206,90 +1272,102 @@
         <v>0</v>
       </c>
       <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
         <v>800</v>
       </c>
-      <c r="V5" s="2">
-        <v>0</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
-      </c>
       <c r="X5" s="2">
         <v>0</v>
       </c>
       <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="2">
         <v>100</v>
       </c>
-      <c r="Z5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>0</v>
-      </c>
       <c r="AB5" s="2">
         <v>0</v>
       </c>
       <c r="AC5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AF5" s="2">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="AE5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>0</v>
-      </c>
       <c r="AG5" s="2">
         <v>0</v>
       </c>
       <c r="AH5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="2">
         <v>2013</v>
       </c>
-      <c r="AI5" s="23">
+      <c r="AK5" s="23">
         <f t="shared" si="6"/>
         <v>500</v>
       </c>
-      <c r="AJ5" s="21">
+      <c r="AL5" s="21">
         <v>500</v>
       </c>
-      <c r="AK5" s="21">
-        <f t="shared" si="7"/>
+      <c r="AM5" s="21">
+        <f t="shared" si="2"/>
         <v>500</v>
       </c>
-      <c r="AL5" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="2">
+      <c r="AN5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="2">
         <f>2*345</f>
         <v>690</v>
       </c>
-      <c r="AN5" s="10">
-        <f t="shared" si="2"/>
+      <c r="AP5" s="10">
+        <f t="shared" si="8"/>
         <v>480</v>
       </c>
-      <c r="AO5" s="27">
-        <f t="shared" si="9"/>
+      <c r="AQ5" s="27">
+        <f>AO5+AP5</f>
         <v>1170</v>
       </c>
-      <c r="AP5" s="15">
-        <f>U5+Y5-AB5-AC5-AD5</f>
+      <c r="AR5" s="15">
+        <f>W5+AA5-AD5-AE5-AF5</f>
         <v>740</v>
       </c>
-      <c r="AQ5">
-        <f>100+0.2*(U5-100)</f>
+      <c r="AS5">
+        <f>100+0.2*(W5-100)</f>
         <v>240</v>
       </c>
-      <c r="AR5" s="10"/>
-      <c r="AS5" s="8"/>
-      <c r="AT5" s="8"/>
+      <c r="AT5" s="10"/>
       <c r="AU5" s="8"/>
-      <c r="AV5" s="11"/>
+      <c r="AV5" s="8">
+        <f t="shared" si="10"/>
+        <v>6.8571428571428568</v>
+      </c>
+      <c r="AW5" s="8">
+        <f>MIN(K5,80)</f>
+        <v>70</v>
+      </c>
+      <c r="AX5" s="11"/>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1321,29 +1399,29 @@
       <c r="J6" s="6">
         <v>80</v>
       </c>
-      <c r="K6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="7">
+      <c r="K6" s="6">
+        <v>70</v>
+      </c>
+      <c r="L6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="7">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M6" s="7">
-        <v>0</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0</v>
-      </c>
       <c r="O6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>0</v>
-      </c>
       <c r="R6" s="7">
         <v>0</v>
       </c>
@@ -1356,13 +1434,13 @@
       <c r="U6" s="7">
         <v>0</v>
       </c>
-      <c r="V6" s="6">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0</v>
-      </c>
-      <c r="X6" s="3">
+      <c r="V6" s="7">
+        <v>0</v>
+      </c>
+      <c r="W6" s="7">
+        <v>0</v>
+      </c>
+      <c r="X6" s="6">
         <v>0</v>
       </c>
       <c r="Y6" s="3">
@@ -1378,65 +1456,76 @@
         <v>0</v>
       </c>
       <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="3">
+      <c r="AF6" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE6" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="3">
-        <v>0</v>
-      </c>
       <c r="AG6" s="3">
         <v>0</v>
       </c>
       <c r="AH6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="3">
         <v>2013</v>
       </c>
-      <c r="AI6" s="24">
+      <c r="AK6" s="24">
         <f t="shared" si="6"/>
         <v>500</v>
       </c>
-      <c r="AJ6" s="22">
+      <c r="AL6" s="22">
         <v>500</v>
       </c>
-      <c r="AK6" s="22">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL6">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="2">
+      <c r="AM6" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="2">
         <f>2*345</f>
         <v>690</v>
       </c>
-      <c r="AN6" s="9">
-        <f t="shared" si="2"/>
+      <c r="AP6" s="9">
+        <f t="shared" si="8"/>
         <v>480</v>
       </c>
-      <c r="AO6" s="28">
+      <c r="AQ6" s="28">
         <f t="shared" si="9"/>
         <v>1170</v>
       </c>
-      <c r="AP6" s="19">
-        <f t="shared" ref="AP6:AP16" si="10">U6-AB6-AC6-AD6</f>
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="20"/>
-      <c r="AS6" s="6"/>
-      <c r="AT6" s="6"/>
+      <c r="AR6" s="19">
+        <f t="shared" ref="AR6:AR16" si="12">W6-AD6-AE6-AF6</f>
+        <v>0</v>
+      </c>
+      <c r="AS6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="20"/>
       <c r="AU6" s="6"/>
-      <c r="AV6" s="11"/>
+      <c r="AV6" s="6">
+        <f t="shared" si="10"/>
+        <v>6.8571428571428568</v>
+      </c>
+      <c r="AW6" s="6">
+        <v>70</v>
+      </c>
+      <c r="AX6" s="11"/>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1468,124 +1557,136 @@
       <c r="J7" s="2">
         <v>80</v>
       </c>
-      <c r="K7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2">
+      <c r="K7" s="2">
+        <v>58</v>
+      </c>
+      <c r="L7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2">
-        <v>1</v>
-      </c>
       <c r="O7" s="2">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>0</v>
-      </c>
       <c r="R7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="2">
         <v>0</v>
       </c>
       <c r="T7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U7" s="2">
+        <v>0</v>
+      </c>
+      <c r="V7" s="2">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2">
         <v>1000</v>
       </c>
-      <c r="V7" s="2">
-        <v>0</v>
-      </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
       <c r="X7" s="2">
         <v>0</v>
       </c>
       <c r="Y7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="2">
         <v>250</v>
       </c>
-      <c r="Z7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="2">
-        <v>0</v>
-      </c>
       <c r="AB7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="2">
         <v>100</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AE7" s="2">
         <f t="shared" si="5"/>
         <v>5.5</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AF7" s="2">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AG7" s="2">
         <v>164</v>
       </c>
-      <c r="AF7" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="2">
-        <v>0</v>
-      </c>
       <c r="AH7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="2">
         <v>2009</v>
       </c>
-      <c r="AI7" s="23">
-        <f>AJ7+AE7</f>
+      <c r="AK7" s="23">
+        <f>AL7+AG7</f>
         <v>848.5</v>
       </c>
-      <c r="AJ7" s="21">
+      <c r="AL7" s="21">
         <v>684.5</v>
       </c>
-      <c r="AK7" s="21">
-        <f t="shared" si="7"/>
+      <c r="AM7" s="21">
+        <f t="shared" si="2"/>
         <v>684.5</v>
       </c>
-      <c r="AL7" s="2">
-        <f>MAX(0.12*P7,0.36)</f>
+      <c r="AN7" s="2">
+        <f>MAX(0.12*R7,0.36)</f>
         <v>0.36</v>
       </c>
-      <c r="AM7" s="2">
-        <f>(1+AL7)*359+(0.6*359)</f>
+      <c r="AO7" s="2">
+        <f>(1+AN7)*359+(0.6*359)</f>
         <v>703.64</v>
       </c>
-      <c r="AN7" s="10">
-        <f t="shared" si="2"/>
-        <v>480</v>
-      </c>
-      <c r="AO7" s="27">
+      <c r="AP7" s="10">
+        <f t="shared" si="8"/>
+        <v>480.00000000000006</v>
+      </c>
+      <c r="AQ7" s="27">
         <f t="shared" si="9"/>
-        <v>1183.6399999999999</v>
-      </c>
-      <c r="AP7" s="15">
-        <f>U7+Y7-AB7-AC7-AD7</f>
+        <v>1183.6400000000001</v>
+      </c>
+      <c r="AR7" s="15">
+        <f>W7+AA7-AD7-AE7-AF7</f>
         <v>944.5</v>
       </c>
-      <c r="AQ7">
+      <c r="AS7">
         <f>100+0.2*(700)+0.1*200</f>
         <v>260</v>
       </c>
-      <c r="AR7" s="10"/>
-      <c r="AS7" s="8"/>
-      <c r="AT7" s="8"/>
+      <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
-      <c r="AV7" s="15"/>
+      <c r="AV7" s="8">
+        <f t="shared" si="10"/>
+        <v>8.2758620689655178</v>
+      </c>
+      <c r="AW7" s="8">
+        <f t="shared" si="11"/>
+        <v>58</v>
+      </c>
+      <c r="AX7" s="15"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1617,43 +1718,43 @@
       <c r="J8" s="3">
         <v>80</v>
       </c>
-      <c r="K8" t="b">
-        <v>1</v>
-      </c>
-      <c r="L8">
+      <c r="K8" s="3">
+        <v>58</v>
+      </c>
+      <c r="L8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M8" s="3">
-        <v>1</v>
-      </c>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
       <c r="O8" s="3">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="P8" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>0</v>
-      </c>
       <c r="R8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" s="3">
         <v>0</v>
       </c>
       <c r="T8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U8" s="3">
         <v>0</v>
       </c>
       <c r="V8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="3">
         <v>0</v>
@@ -1674,66 +1775,78 @@
         <v>0</v>
       </c>
       <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD8" s="3">
+      <c r="AF8" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE8" s="3">
+      <c r="AG8" s="3">
         <v>164</v>
       </c>
-      <c r="AF8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="3">
-        <v>0</v>
-      </c>
       <c r="AH8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="3">
         <v>2009</v>
       </c>
-      <c r="AI8" s="24">
+      <c r="AK8" s="24">
         <f t="shared" si="6"/>
         <v>848.5</v>
       </c>
-      <c r="AJ8" s="22">
+      <c r="AL8" s="22">
         <v>684.5</v>
       </c>
-      <c r="AK8" s="22">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL8">
-        <f>MAX(0.12*P8,0.36)</f>
+      <c r="AM8" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <f>MAX(0.12*R8,0.36)</f>
         <v>0.36</v>
       </c>
-      <c r="AM8" s="7">
-        <f>(1+AL8)*359+(0.6*359)</f>
+      <c r="AO8" s="7">
+        <f>(1+AN8)*359+(0.6*359)</f>
         <v>703.64</v>
       </c>
-      <c r="AN8" s="9">
-        <f t="shared" si="2"/>
-        <v>480</v>
-      </c>
-      <c r="AO8" s="29">
+      <c r="AP8" s="9">
+        <f t="shared" si="8"/>
+        <v>480.00000000000006</v>
+      </c>
+      <c r="AQ8" s="29">
         <f t="shared" si="9"/>
-        <v>1183.6399999999999</v>
-      </c>
-      <c r="AP8" s="17">
+        <v>1183.6400000000001</v>
+      </c>
+      <c r="AR8" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AS8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="9"/>
+      <c r="AU8" s="3"/>
+      <c r="AV8" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="9"/>
-      <c r="AS8" s="3"/>
-      <c r="AT8" s="3"/>
-      <c r="AU8" s="3"/>
-      <c r="AV8" s="17"/>
+        <v>8.2758620689655178</v>
+      </c>
+      <c r="AW8" s="3">
+        <f t="shared" si="11"/>
+        <v>58</v>
+      </c>
+      <c r="AX8" s="17"/>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>4</v>
       </c>
@@ -1765,43 +1878,43 @@
       <c r="J9" s="2">
         <v>120</v>
       </c>
-      <c r="K9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="2">
+      <c r="K9" s="2">
+        <v>110</v>
+      </c>
+      <c r="L9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2">
-        <v>2</v>
-      </c>
       <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="2">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="P9" s="2">
+      <c r="R9" s="2">
         <v>3</v>
       </c>
-      <c r="Q9" s="2">
-        <v>0</v>
-      </c>
-      <c r="R9" s="2">
-        <v>2</v>
-      </c>
       <c r="S9" s="2">
         <v>0</v>
       </c>
       <c r="T9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U9" s="2">
         <v>0</v>
       </c>
       <c r="V9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9" s="2">
         <v>0</v>
@@ -1822,66 +1935,78 @@
         <v>0</v>
       </c>
       <c r="AC9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AF9" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AG9" s="2">
         <f>3*154</f>
         <v>462</v>
       </c>
-      <c r="AF9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="2">
-        <v>0</v>
-      </c>
       <c r="AH9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="2">
         <v>2006</v>
       </c>
-      <c r="AI9" s="23">
+      <c r="AK9" s="23">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AJ9" s="21">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="21">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="2">
+      <c r="AL9" s="21">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="2">
         <f>345*0.9*2+345*0.6+345*0.7*2</f>
         <v>1311</v>
       </c>
-      <c r="AN9" s="10">
-        <f t="shared" si="2"/>
-        <v>970</v>
-      </c>
-      <c r="AO9" s="27">
+      <c r="AP9" s="10">
+        <f t="shared" si="8"/>
+        <v>925.90909090909088</v>
+      </c>
+      <c r="AQ9" s="27">
         <f t="shared" si="9"/>
-        <v>2281</v>
-      </c>
-      <c r="AP9" s="15">
+        <v>2236.909090909091</v>
+      </c>
+      <c r="AR9" s="15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AS9" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="10"/>
+      <c r="AU9" s="16"/>
+      <c r="AV9" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="10"/>
-      <c r="AS9" s="16"/>
-      <c r="AT9" s="8"/>
-      <c r="AU9" s="2"/>
-      <c r="AV9" s="11"/>
+        <v>8.8181818181818183</v>
+      </c>
+      <c r="AW9" s="2">
+        <f t="shared" si="11"/>
+        <v>105</v>
+      </c>
+      <c r="AX9" s="11"/>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1913,43 +2038,43 @@
       <c r="J10" s="4">
         <v>120</v>
       </c>
-      <c r="K10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10">
+      <c r="K10" s="3">
+        <v>110</v>
+      </c>
+      <c r="L10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M10" s="3">
-        <v>1</v>
-      </c>
-      <c r="N10" s="3">
-        <v>2</v>
-      </c>
       <c r="O10" s="3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="P10" s="3">
+      <c r="R10" s="3">
         <v>3</v>
       </c>
-      <c r="Q10" s="3">
-        <v>0</v>
-      </c>
-      <c r="R10" s="3">
-        <v>2</v>
-      </c>
       <c r="S10" s="3">
         <v>0</v>
       </c>
       <c r="T10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U10" s="3">
         <v>0</v>
       </c>
       <c r="V10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" s="3">
         <v>0</v>
@@ -1970,66 +2095,78 @@
         <v>0</v>
       </c>
       <c r="AC10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="3">
+      <c r="AF10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE10" s="3">
-        <f t="shared" ref="AE10:AE13" si="11">3*154</f>
+      <c r="AG10" s="3">
+        <f t="shared" ref="AG10:AG13" si="13">3*154</f>
         <v>462</v>
       </c>
-      <c r="AF10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="4">
+      <c r="AH10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="4">
         <v>2006</v>
       </c>
-      <c r="AI10" s="12">
+      <c r="AK10" s="12">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AJ10" s="22">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="22">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL10">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="3">
-        <f t="shared" ref="AM10:AM13" si="12">345*0.9*2+345*0.6+345*0.7*2</f>
+      <c r="AL10" s="22">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="3">
+        <f t="shared" ref="AO10:AO13" si="14">345*0.9*2+345*0.6+345*0.7*2</f>
         <v>1311</v>
       </c>
-      <c r="AN10" s="9">
-        <f t="shared" si="2"/>
-        <v>970</v>
-      </c>
-      <c r="AO10" s="29">
+      <c r="AP10" s="9">
+        <f t="shared" si="8"/>
+        <v>925.90909090909088</v>
+      </c>
+      <c r="AQ10" s="29">
         <f t="shared" si="9"/>
-        <v>2281</v>
-      </c>
-      <c r="AP10" s="17">
+        <v>2236.909090909091</v>
+      </c>
+      <c r="AR10" s="17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AS10" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="18"/>
+      <c r="AV10" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="9"/>
-      <c r="AS10" s="18"/>
-      <c r="AT10" s="3"/>
-      <c r="AU10" s="4"/>
-      <c r="AV10" s="11"/>
+        <v>8.8181818181818183</v>
+      </c>
+      <c r="AW10" s="4">
+        <f t="shared" si="11"/>
+        <v>105</v>
+      </c>
+      <c r="AX10" s="11"/>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2061,43 +2198,43 @@
       <c r="J11" s="4">
         <v>120</v>
       </c>
-      <c r="K11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="K11" s="3">
+        <v>110</v>
+      </c>
+      <c r="L11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M11" s="3">
-        <v>1</v>
-      </c>
-      <c r="N11" s="3">
-        <v>2</v>
-      </c>
       <c r="O11" s="3">
+        <v>1</v>
+      </c>
+      <c r="P11" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="P11" s="3">
+      <c r="R11" s="3">
         <v>3</v>
       </c>
-      <c r="Q11" s="3">
-        <v>0</v>
-      </c>
-      <c r="R11" s="3">
-        <v>2</v>
-      </c>
       <c r="S11" s="3">
         <v>0</v>
       </c>
       <c r="T11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11" s="3">
         <v>0</v>
       </c>
       <c r="V11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11" s="3">
         <v>0</v>
@@ -2118,65 +2255,78 @@
         <v>0</v>
       </c>
       <c r="AC11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="3">
+      <c r="AF11" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE11" s="3">
-        <f t="shared" si="11"/>
+      <c r="AG11" s="3">
+        <f t="shared" si="13"/>
         <v>462</v>
       </c>
-      <c r="AF11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="4">
+      <c r="AH11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="4">
         <v>2006</v>
       </c>
-      <c r="AI11" s="12">
+      <c r="AK11" s="12">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AJ11" s="22">
-        <v>0</v>
-      </c>
-      <c r="AK11" s="22">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL11">
-        <v>0</v>
-      </c>
-      <c r="AM11" s="3">
+      <c r="AL11" s="22">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="3">
+        <f t="shared" si="14"/>
+        <v>1311</v>
+      </c>
+      <c r="AP11" s="9">
+        <f t="shared" si="8"/>
+        <v>925.90909090909088</v>
+      </c>
+      <c r="AQ11" s="29">
+        <f t="shared" si="9"/>
+        <v>2236.909090909091</v>
+      </c>
+      <c r="AR11" s="11">
         <f t="shared" si="12"/>
-        <v>1311</v>
-      </c>
-      <c r="AN11" s="9">
-        <f t="shared" si="2"/>
-        <v>970</v>
-      </c>
-      <c r="AO11" s="29">
-        <f t="shared" si="9"/>
-        <v>2281</v>
-      </c>
-      <c r="AP11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="9"/>
+      <c r="AU11" s="5"/>
+      <c r="AV11" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ11">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="9"/>
-      <c r="AS11" s="5"/>
-      <c r="AT11" s="3"/>
-      <c r="AV11" s="11"/>
+        <v>8.8181818181818183</v>
+      </c>
+      <c r="AW11">
+        <f t="shared" si="11"/>
+        <v>105</v>
+      </c>
+      <c r="AX11" s="11"/>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -2208,43 +2358,43 @@
       <c r="J12" s="4">
         <v>120</v>
       </c>
-      <c r="K12" t="b">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="K12" s="3">
+        <v>110</v>
+      </c>
+      <c r="L12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M12" s="3">
-        <v>1</v>
-      </c>
-      <c r="N12" s="3">
-        <v>2</v>
-      </c>
       <c r="O12" s="3">
+        <v>1</v>
+      </c>
+      <c r="P12" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="P12" s="3">
+      <c r="R12" s="3">
         <v>3</v>
       </c>
-      <c r="Q12" s="3">
-        <v>0</v>
-      </c>
-      <c r="R12" s="3">
-        <v>2</v>
-      </c>
       <c r="S12" s="3">
         <v>0</v>
       </c>
       <c r="T12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12" s="3">
         <v>0</v>
       </c>
       <c r="V12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W12" s="3">
         <v>0</v>
@@ -2265,65 +2415,78 @@
         <v>0</v>
       </c>
       <c r="AC12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD12" s="3">
+      <c r="AF12" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE12" s="3">
-        <f t="shared" si="11"/>
+      <c r="AG12" s="3">
+        <f t="shared" si="13"/>
         <v>462</v>
       </c>
-      <c r="AF12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="4">
+      <c r="AH12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="4">
         <v>2006</v>
       </c>
-      <c r="AI12" s="12">
+      <c r="AK12" s="12">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AJ12" s="22">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="22">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL12" s="25">
-        <v>0</v>
-      </c>
-      <c r="AM12" s="3">
+      <c r="AL12" s="22">
+        <v>0</v>
+      </c>
+      <c r="AM12" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN12" s="25">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="3">
+        <f t="shared" si="14"/>
+        <v>1311</v>
+      </c>
+      <c r="AP12" s="9">
+        <f t="shared" si="8"/>
+        <v>925.90909090909088</v>
+      </c>
+      <c r="AQ12" s="29">
+        <f t="shared" si="9"/>
+        <v>2236.909090909091</v>
+      </c>
+      <c r="AR12" s="11">
         <f t="shared" si="12"/>
-        <v>1311</v>
-      </c>
-      <c r="AN12" s="9">
-        <f t="shared" si="2"/>
-        <v>970</v>
-      </c>
-      <c r="AO12" s="29">
-        <f t="shared" si="9"/>
-        <v>2281</v>
-      </c>
-      <c r="AP12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS12">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="5"/>
+      <c r="AV12" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ12">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="9"/>
-      <c r="AS12" s="5"/>
-      <c r="AT12" s="3"/>
-      <c r="AV12" s="11"/>
+        <v>8.8181818181818183</v>
+      </c>
+      <c r="AW12">
+        <f t="shared" si="11"/>
+        <v>105</v>
+      </c>
+      <c r="AX12" s="11"/>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2355,43 +2518,43 @@
       <c r="J13" s="4">
         <v>120</v>
       </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="K13" s="3">
+        <v>110</v>
+      </c>
+      <c r="L13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M13" s="3">
-        <v>1</v>
-      </c>
-      <c r="N13" s="3">
-        <v>2</v>
-      </c>
       <c r="O13" s="3">
+        <v>1</v>
+      </c>
+      <c r="P13" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="3">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="P13" s="3">
+      <c r="R13" s="3">
         <v>3</v>
       </c>
-      <c r="Q13" s="3">
-        <v>0</v>
-      </c>
-      <c r="R13" s="3">
-        <v>2</v>
-      </c>
       <c r="S13" s="3">
         <v>0</v>
       </c>
       <c r="T13" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U13" s="3">
         <v>0</v>
       </c>
       <c r="V13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W13" s="3">
         <v>0</v>
@@ -2412,65 +2575,78 @@
         <v>0</v>
       </c>
       <c r="AC13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AD13" s="3">
+      <c r="AF13" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE13" s="3">
-        <f t="shared" si="11"/>
+      <c r="AG13" s="3">
+        <f t="shared" si="13"/>
         <v>462</v>
       </c>
-      <c r="AF13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="4">
+      <c r="AH13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="4">
         <v>2006</v>
       </c>
-      <c r="AI13" s="12">
+      <c r="AK13" s="12">
         <f t="shared" si="6"/>
         <v>462</v>
       </c>
-      <c r="AJ13" s="22">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="22">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL13" s="25">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="3">
+      <c r="AL13" s="22">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN13" s="25">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="3">
+        <f t="shared" si="14"/>
+        <v>1311</v>
+      </c>
+      <c r="AP13" s="9">
+        <f t="shared" si="8"/>
+        <v>925.90909090909088</v>
+      </c>
+      <c r="AQ13" s="29">
+        <f t="shared" si="9"/>
+        <v>2236.909090909091</v>
+      </c>
+      <c r="AR13" s="11">
         <f t="shared" si="12"/>
-        <v>1311</v>
-      </c>
-      <c r="AN13" s="9">
-        <f t="shared" si="2"/>
-        <v>970</v>
-      </c>
-      <c r="AO13" s="29">
-        <f t="shared" si="9"/>
-        <v>2281</v>
-      </c>
-      <c r="AP13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS13">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="9"/>
+      <c r="AU13" s="5"/>
+      <c r="AV13" s="3">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ13">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="9"/>
-      <c r="AS13" s="5"/>
-      <c r="AT13" s="3"/>
-      <c r="AV13" s="11"/>
+        <v>8.8181818181818183</v>
+      </c>
+      <c r="AW13">
+        <f t="shared" si="11"/>
+        <v>105</v>
+      </c>
+      <c r="AX13" s="11"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2502,19 +2678,19 @@
       <c r="J14" s="2">
         <v>110</v>
       </c>
-      <c r="K14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" s="2">
+      <c r="K14" s="2">
+        <v>105</v>
+      </c>
+      <c r="L14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
         <v>3</v>
       </c>
-      <c r="M14" s="8">
-        <v>0</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0</v>
-      </c>
-      <c r="O14" s="2">
+      <c r="O14" s="8">
         <v>0</v>
       </c>
       <c r="P14" s="2">
@@ -2533,14 +2709,14 @@
         <v>0</v>
       </c>
       <c r="U14" s="2">
+        <v>0</v>
+      </c>
+      <c r="V14" s="2">
+        <v>0</v>
+      </c>
+      <c r="W14" s="2">
         <v>1700</v>
       </c>
-      <c r="V14" s="2">
-        <v>0</v>
-      </c>
-      <c r="W14" s="2">
-        <v>0</v>
-      </c>
       <c r="X14" s="2">
         <v>0</v>
       </c>
@@ -2554,66 +2730,80 @@
         <v>0</v>
       </c>
       <c r="AB14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="2">
         <v>200</v>
       </c>
-      <c r="AC14" s="2">
+      <c r="AE14" s="2">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="AD14" s="2">
+      <c r="AF14" s="2">
         <f t="shared" si="1"/>
         <v>340</v>
       </c>
-      <c r="AE14" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="2">
-        <v>0</v>
-      </c>
       <c r="AG14" s="2">
         <v>0</v>
       </c>
       <c r="AH14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="2">
         <v>2011</v>
       </c>
-      <c r="AI14" s="21">
-        <f t="shared" ref="AI14:AI16" si="13">AJ14+AE14</f>
+      <c r="AK14" s="21">
+        <f t="shared" ref="AK14:AK16" si="15">AL14+AG14</f>
         <v>1289</v>
       </c>
-      <c r="AJ14" s="21">
-        <f>AK14+AK16</f>
+      <c r="AL14" s="21">
+        <f>AM14+AM16</f>
         <v>1289</v>
       </c>
-      <c r="AK14" s="21">
-        <f t="shared" si="7"/>
+      <c r="AM14" s="21">
+        <f t="shared" si="2"/>
         <v>849</v>
       </c>
-      <c r="AL14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM14" s="8">
+      <c r="AN14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="8">
         <f>2*328+291</f>
         <v>947</v>
       </c>
-      <c r="AN14" s="2">
-        <f t="shared" si="2"/>
-        <v>830</v>
-      </c>
-      <c r="AO14" s="27">
+      <c r="AP14" s="10">
+        <f t="shared" si="8"/>
+        <v>592.85714285714289</v>
+      </c>
+      <c r="AQ14" s="27">
         <f t="shared" si="9"/>
-        <v>1777</v>
-      </c>
-      <c r="AP14" s="2">
-        <f t="shared" si="10"/>
+        <v>1539.8571428571429</v>
+      </c>
+      <c r="AR14" s="2">
+        <f t="shared" si="12"/>
         <v>1149</v>
       </c>
-      <c r="AQ14">
+      <c r="AS14">
         <f>100+0.2*900+0.1*200</f>
         <v>300</v>
       </c>
-      <c r="AR14" s="9"/>
+      <c r="AT14" s="9"/>
+      <c r="AV14">
+        <f t="shared" si="10"/>
+        <v>7.9047619047619051</v>
+      </c>
+      <c r="AW14">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -2645,18 +2835,18 @@
       <c r="J15">
         <v>110</v>
       </c>
-      <c r="K15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15">
+      <c r="K15" s="3">
+        <v>105</v>
+      </c>
+      <c r="L15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15">
         <v>3</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
       <c r="O15">
         <v>0</v>
       </c>
@@ -2675,10 +2865,10 @@
       <c r="T15">
         <v>0</v>
       </c>
-      <c r="U15" s="3">
-        <v>0</v>
-      </c>
-      <c r="V15" s="3">
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
         <v>0</v>
       </c>
       <c r="W15" s="3">
@@ -2703,57 +2893,71 @@
         <v>0</v>
       </c>
       <c r="AD15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE15">
-        <v>0</v>
-      </c>
-      <c r="AF15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH15" s="2">
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="2">
         <v>2011</v>
       </c>
-      <c r="AI15" s="1">
-        <f>AJ15+AE15</f>
+      <c r="AK15" s="1">
+        <f>AL15+AG15</f>
         <v>1289</v>
       </c>
-      <c r="AJ15" s="1">
+      <c r="AL15" s="1">
         <v>1289</v>
       </c>
-      <c r="AK15" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL15" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM15" s="8">
+      <c r="AM15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="8">
         <f>2*328+291</f>
         <v>947</v>
       </c>
-      <c r="AN15">
-        <f t="shared" ref="AN15:AN16" si="14">I15+J15</f>
-        <v>830</v>
-      </c>
-      <c r="AO15" s="26">
+      <c r="AP15" s="9">
+        <f t="shared" si="8"/>
+        <v>592.85714285714289</v>
+      </c>
+      <c r="AQ15" s="26">
         <f t="shared" si="9"/>
-        <v>1777</v>
-      </c>
-      <c r="AP15">
+        <v>1539.8571428571429</v>
+      </c>
+      <c r="AR15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="9"/>
+      <c r="AV15">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AQ15">
-        <v>0</v>
-      </c>
-      <c r="AR15" s="9"/>
+        <v>7.9047619047619051</v>
+      </c>
+      <c r="AW15">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -2785,18 +2989,18 @@
       <c r="J16">
         <v>110</v>
       </c>
-      <c r="K16" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16">
+      <c r="K16" s="3">
+        <v>105</v>
+      </c>
+      <c r="L16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16">
         <v>3</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
       <c r="O16">
         <v>0</v>
       </c>
@@ -2815,15 +3019,15 @@
       <c r="T16">
         <v>0</v>
       </c>
-      <c r="U16" s="3">
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16" s="3">
         <v>800</v>
       </c>
-      <c r="V16" s="3">
-        <v>0</v>
-      </c>
-      <c r="W16" s="3">
-        <v>0</v>
-      </c>
       <c r="X16" s="3">
         <v>0</v>
       </c>
@@ -2843,58 +3047,72 @@
         <v>0</v>
       </c>
       <c r="AD16" s="3">
-        <f>0.15*U16</f>
+        <v>0</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="3">
+        <f>0.15*W16</f>
         <v>120</v>
       </c>
-      <c r="AE16">
-        <v>0</v>
-      </c>
-      <c r="AF16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH16" s="2">
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="2">
         <v>2011</v>
       </c>
-      <c r="AI16" s="1">
-        <f t="shared" si="13"/>
+      <c r="AK16" s="1">
+        <f t="shared" si="15"/>
         <v>1289</v>
       </c>
-      <c r="AJ16" s="1">
+      <c r="AL16" s="1">
         <v>1289</v>
       </c>
-      <c r="AK16" s="1">
-        <f t="shared" si="7"/>
+      <c r="AM16" s="1">
+        <f t="shared" si="2"/>
         <v>440</v>
       </c>
-      <c r="AL16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM16" s="8">
+      <c r="AN16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="8">
         <f>2*328+291</f>
         <v>947</v>
       </c>
-      <c r="AN16">
-        <f t="shared" si="14"/>
-        <v>830</v>
-      </c>
-      <c r="AO16" s="26">
+      <c r="AP16" s="9">
+        <f t="shared" si="8"/>
+        <v>592.85714285714289</v>
+      </c>
+      <c r="AQ16" s="26">
         <f t="shared" si="9"/>
-        <v>1777</v>
-      </c>
-      <c r="AP16">
+        <v>1539.8571428571429</v>
+      </c>
+      <c r="AR16">
+        <f t="shared" si="12"/>
+        <v>680</v>
+      </c>
+      <c r="AS16">
+        <f>100+0.2*(W16-100)</f>
+        <v>240</v>
+      </c>
+      <c r="AT16" s="9"/>
+      <c r="AV16">
         <f t="shared" si="10"/>
-        <v>680</v>
-      </c>
-      <c r="AQ16">
-        <f>100+0.2*(U16-100)</f>
-        <v>240</v>
-      </c>
-      <c r="AR16" s="9"/>
+        <v>7.9047619047619051</v>
+      </c>
+      <c r="AW16">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
     </row>
-    <row r="17" spans="1:45" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -2926,45 +3144,45 @@
       <c r="J17" s="2">
         <v>80</v>
       </c>
-      <c r="K17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L17" s="2">
-        <v>1</v>
-      </c>
-      <c r="M17" s="2">
+      <c r="K17" s="2">
+        <v>60</v>
+      </c>
+      <c r="L17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2" t="b">
         <v>1</v>
       </c>
       <c r="N17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P17" s="2">
         <v>2</v>
       </c>
       <c r="Q17" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" s="2">
+        <v>1</v>
+      </c>
+      <c r="V17" s="2">
+        <v>0</v>
+      </c>
+      <c r="W17" s="2">
         <v>800</v>
       </c>
-      <c r="V17" s="2">
-        <v>0</v>
-      </c>
-      <c r="W17" s="2">
-        <v>0</v>
-      </c>
       <c r="X17" s="2">
         <v>0</v>
       </c>
@@ -2984,60 +3202,74 @@
         <v>0</v>
       </c>
       <c r="AD17" s="2">
-        <f>0.17*U17</f>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="2">
+        <f>0.17*W17</f>
         <v>136</v>
       </c>
-      <c r="AE17" s="2">
+      <c r="AG17" s="2">
         <f>2*194</f>
         <v>388</v>
       </c>
-      <c r="AF17" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="2">
-        <v>0</v>
-      </c>
       <c r="AH17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="2">
         <v>2019</v>
       </c>
-      <c r="AI17" s="1">
-        <f>AJ17+AE17+212+160</f>
+      <c r="AK17" s="1">
+        <f>AL17+AG17+212+160</f>
         <v>1184</v>
       </c>
-      <c r="AJ17" s="21">
-        <f>AK17+AK19</f>
+      <c r="AL17" s="21">
+        <f>AM17+AM19</f>
         <v>424</v>
       </c>
-      <c r="AK17" s="1">
-        <f t="shared" si="7"/>
+      <c r="AM17" s="1">
+        <f t="shared" si="2"/>
         <v>424</v>
       </c>
-      <c r="AL17" s="3">
+      <c r="AN17" s="3">
         <v>0.36</v>
       </c>
-      <c r="AM17">
-        <f>(1+AL17)*424+(245+302)</f>
+      <c r="AO17">
+        <f>(1+AN17)*424+(245+302)</f>
         <v>1123.6399999999999</v>
       </c>
-      <c r="AN17">
-        <f t="shared" ref="AN17:AN19" si="15">I17+J17</f>
+      <c r="AP17" s="9">
+        <f t="shared" si="8"/>
         <v>518</v>
       </c>
-      <c r="AO17" s="26">
-        <f>AM17+AN17</f>
+      <c r="AQ17" s="26">
+        <f>AO17+AP17</f>
         <v>1641.6399999999999</v>
       </c>
-      <c r="AP17">
-        <f>U17-AB17-AC17-AD17</f>
+      <c r="AR17">
+        <f>W17-AD17-AE17-AF17</f>
         <v>664</v>
       </c>
-      <c r="AQ17">
-        <f t="shared" ref="AQ17" si="16">100+0.2*(U17-100)</f>
+      <c r="AS17">
+        <f t="shared" ref="AS17" si="16">100+0.2*(W17-100)</f>
         <v>240</v>
       </c>
-      <c r="AR17" s="10"/>
+      <c r="AT17" s="10"/>
+      <c r="AV17" s="2">
+        <f t="shared" si="10"/>
+        <v>8.6333333333333329</v>
+      </c>
+      <c r="AW17" s="2">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>6</v>
       </c>
@@ -3069,40 +3301,40 @@
       <c r="J18" s="3">
         <v>80</v>
       </c>
-      <c r="K18" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
+      <c r="K18" s="3">
+        <v>60</v>
+      </c>
+      <c r="L18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="N18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P18">
         <v>2</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18" s="3">
-        <v>0</v>
-      </c>
-      <c r="V18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
         <v>0</v>
       </c>
       <c r="W18" s="3">
@@ -3130,53 +3362,67 @@
         <v>0</v>
       </c>
       <c r="AE18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="3">
         <v>388</v>
       </c>
-      <c r="AF18" s="3">
+      <c r="AH18" s="3">
         <v>212</v>
       </c>
-      <c r="AG18" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH18" s="3">
+      <c r="AI18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="3">
         <v>2019</v>
       </c>
-      <c r="AI18" s="1">
-        <f>AJ18+AE18+212+160</f>
+      <c r="AK18" s="1">
+        <f>AL18+AG18+212+160</f>
         <v>1184</v>
       </c>
-      <c r="AJ18" s="1">
+      <c r="AL18" s="1">
         <v>424</v>
       </c>
-      <c r="AK18" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL18" s="3">
+      <c r="AM18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN18" s="3">
         <v>0.36</v>
       </c>
-      <c r="AM18">
-        <f t="shared" ref="AM18:AM19" si="17">(1+AL18)*424+(245+302)</f>
+      <c r="AO18">
+        <f t="shared" ref="AO18:AO19" si="17">(1+AN18)*424+(245+302)</f>
         <v>1123.6399999999999</v>
       </c>
-      <c r="AN18">
-        <f t="shared" si="15"/>
+      <c r="AP18" s="9">
+        <f t="shared" si="8"/>
         <v>518</v>
       </c>
-      <c r="AO18" s="26">
-        <f t="shared" ref="AO18:AO19" si="18">AM18+AN18</f>
+      <c r="AQ18" s="26">
+        <f t="shared" ref="AQ18:AQ19" si="18">AO18+AP18</f>
         <v>1641.6399999999999</v>
       </c>
-      <c r="AP18">
-        <f t="shared" ref="AP18:AP19" si="19">U18-AB18-AC18-AD18</f>
-        <v>0</v>
-      </c>
-      <c r="AQ18">
-        <v>0</v>
-      </c>
-      <c r="AR18" s="9"/>
+      <c r="AR18">
+        <f t="shared" ref="AR18:AR19" si="19">W18-AD18-AE18-AF18</f>
+        <v>0</v>
+      </c>
+      <c r="AS18">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="9"/>
+      <c r="AV18">
+        <f t="shared" si="10"/>
+        <v>8.6333333333333329</v>
+      </c>
+      <c r="AW18">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -3199,7 +3445,7 @@
         <v>3</v>
       </c>
       <c r="H19">
-        <f>AH19-G19</f>
+        <f>AJ19-G19</f>
         <v>2016</v>
       </c>
       <c r="I19" s="3">
@@ -3208,40 +3454,40 @@
       <c r="J19" s="3">
         <v>80</v>
       </c>
-      <c r="K19" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
+      <c r="K19" s="3">
+        <v>60</v>
+      </c>
+      <c r="L19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="N19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P19">
         <v>2</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19" s="3">
-        <v>0</v>
-      </c>
-      <c r="V19" s="3">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="V19">
         <v>0</v>
       </c>
       <c r="W19" s="3">
@@ -3269,53 +3515,67 @@
         <v>0</v>
       </c>
       <c r="AE19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="3">
         <v>388</v>
       </c>
-      <c r="AF19" s="3">
+      <c r="AH19" s="3">
         <v>160</v>
       </c>
-      <c r="AG19" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH19" s="3">
+      <c r="AI19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="3">
         <v>2019</v>
       </c>
-      <c r="AI19" s="1">
-        <f>AJ19+AE19+212+160</f>
+      <c r="AK19" s="1">
+        <f>AL19+AG19+212+160</f>
         <v>1184</v>
       </c>
-      <c r="AJ19" s="1">
+      <c r="AL19" s="1">
         <v>424</v>
       </c>
-      <c r="AK19" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL19" s="3">
+      <c r="AM19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN19" s="3">
         <v>0.36</v>
       </c>
-      <c r="AM19">
+      <c r="AO19">
         <f t="shared" si="17"/>
         <v>1123.6399999999999</v>
       </c>
-      <c r="AN19">
-        <f t="shared" si="15"/>
+      <c r="AP19" s="9">
+        <f t="shared" si="8"/>
         <v>518</v>
       </c>
-      <c r="AO19" s="26">
+      <c r="AQ19" s="26">
         <f t="shared" si="18"/>
         <v>1641.6399999999999</v>
       </c>
-      <c r="AP19">
+      <c r="AR19">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AQ19">
-        <v>0</v>
-      </c>
-      <c r="AR19" s="9"/>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="9"/>
+      <c r="AV19">
+        <f t="shared" si="10"/>
+        <v>8.6333333333333329</v>
+      </c>
+      <c r="AW19">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>7</v>
       </c>
@@ -3338,7 +3598,7 @@
         <v>75</v>
       </c>
       <c r="H20" s="2">
-        <f>AH20-G20</f>
+        <f>AJ20-G20</f>
         <v>1935</v>
       </c>
       <c r="I20" s="2">
@@ -3347,17 +3607,17 @@
       <c r="J20" s="2">
         <v>100</v>
       </c>
-      <c r="K20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" s="2">
-        <v>2</v>
-      </c>
-      <c r="M20" s="2">
+      <c r="K20" s="2">
+        <v>40</v>
+      </c>
+      <c r="L20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N20" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O20" s="2">
         <v>0</v>
@@ -3383,16 +3643,16 @@
       <c r="V20" s="2">
         <v>0</v>
       </c>
-      <c r="W20" s="8">
-        <f>AG20/12</f>
+      <c r="W20" s="2">
+        <v>0</v>
+      </c>
+      <c r="X20" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="8">
+        <f>AI20/12</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="X20" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="2">
-        <v>0</v>
-      </c>
       <c r="Z20" s="2">
         <v>0</v>
       </c>
@@ -3415,54 +3675,68 @@
         <v>0</v>
       </c>
       <c r="AG20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="2">
         <v>800</v>
       </c>
-      <c r="AH20" s="2">
+      <c r="AJ20" s="2">
         <v>2010</v>
       </c>
-      <c r="AI20" s="1">
-        <f>AJ20+AE20</f>
+      <c r="AK20" s="1">
+        <f>AL20+AG20</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AJ20" s="1">
-        <f>AK20+AK21</f>
+      <c r="AL20" s="1">
+        <f>AM20+AM21</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AK20" s="1">
-        <f>$AP20-$AQ20</f>
+      <c r="AM20" s="1">
+        <f t="shared" si="2"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="AL20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM20">
+      <c r="AN20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO20">
         <f>2*359*0.9</f>
         <v>646.20000000000005</v>
       </c>
-      <c r="AN20">
-        <f t="shared" ref="AN20:AN21" si="20">I20+J20</f>
-        <v>600</v>
-      </c>
-      <c r="AO20" s="26">
-        <f>IF(AG20/0.025&gt;$AR$20+$AR$21,0,AM20+AN20)</f>
-        <v>1246.2</v>
-      </c>
-      <c r="AP20">
-        <f>W20+U20-AB20-AC20-AD20</f>
+      <c r="AP20" s="9">
+        <f t="shared" si="8"/>
+        <v>400</v>
+      </c>
+      <c r="AQ20" s="26">
+        <f>IF(AI20/0.025&gt;$AT$20+$AT$21,0,AO20+AP20)</f>
+        <v>1046.2</v>
+      </c>
+      <c r="AR20">
+        <f>Y20+W20-AD20-AE20-AF20</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AQ20">
-        <v>0</v>
-      </c>
-      <c r="AR20" s="9">
-        <f>MIN(MAX(3100,520*G20),AS20)</f>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="9">
+        <f>MIN(MAX(3100,520*G20),AU20)</f>
         <v>33800</v>
       </c>
-      <c r="AS20">
+      <c r="AU20">
         <v>33800</v>
       </c>
+      <c r="AV20">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="AW20">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>7</v>
       </c>
@@ -3485,7 +3759,7 @@
         <v>50</v>
       </c>
       <c r="H21" s="3">
-        <f>AH21-G21</f>
+        <f>AJ21-G21</f>
         <v>1960</v>
       </c>
       <c r="I21" s="3">
@@ -3494,17 +3768,17 @@
       <c r="J21" s="3">
         <v>100</v>
       </c>
-      <c r="K21" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L21" s="3">
-        <v>2</v>
-      </c>
-      <c r="M21" s="3">
+      <c r="K21" s="3">
+        <v>40</v>
+      </c>
+      <c r="L21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="N21" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O21" s="3">
         <v>0</v>
@@ -3561,85 +3835,99 @@
         <v>0</v>
       </c>
       <c r="AG21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="3">
         <v>800</v>
       </c>
-      <c r="AH21" s="3">
+      <c r="AJ21" s="3">
         <v>2010</v>
       </c>
-      <c r="AI21" s="1">
-        <f t="shared" ref="AI21" si="21">AJ21+AE21</f>
+      <c r="AK21" s="1">
+        <f t="shared" ref="AK21" si="20">AL21+AG21</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AJ21" s="1">
-        <f>AK21+AK20</f>
+      <c r="AL21" s="1">
+        <f>AM21+AM20</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="AK21" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AL21" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM21">
+      <c r="AM21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO21">
         <f>2*359*0.9</f>
         <v>646.20000000000005</v>
       </c>
-      <c r="AN21">
-        <f t="shared" si="20"/>
-        <v>600</v>
-      </c>
-      <c r="AO21" s="26">
-        <f>IF(AG21/0.025&gt;$AR$20+$AR$21,0,AM21+AN21)</f>
-        <v>1246.2</v>
-      </c>
-      <c r="AP21">
-        <f>W21+U21-AB21-AC21-AD21</f>
-        <v>0</v>
-      </c>
-      <c r="AQ21">
-        <v>0</v>
-      </c>
-      <c r="AR21" s="9">
-        <f>MIN(MAX(3100,150*G21),AS21)</f>
+      <c r="AP21" s="9">
+        <f t="shared" si="8"/>
+        <v>400</v>
+      </c>
+      <c r="AQ21" s="26">
+        <f>IF(AI21/0.025&gt;$AT$20+$AT$21,0,AO21+AP21)</f>
+        <v>1046.2</v>
+      </c>
+      <c r="AR21">
+        <f>Y21+W21-AD21-AE21-AF21</f>
+        <v>0</v>
+      </c>
+      <c r="AS21">
+        <v>0</v>
+      </c>
+      <c r="AT21" s="9">
+        <f>MIN(MAX(3100,150*G21),AU21)</f>
         <v>7500</v>
       </c>
-      <c r="AS21">
+      <c r="AU21">
         <v>10050</v>
       </c>
+      <c r="AV21">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="AW21">
+        <f t="shared" si="11"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AL22" s="25"/>
-      <c r="AO22" s="9"/>
-      <c r="AR22" s="9"/>
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AN22" s="25"/>
+      <c r="AQ22" s="9"/>
+      <c r="AT22" s="9"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AO23" s="9"/>
-      <c r="AR23" s="9"/>
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AQ23" s="9"/>
+      <c r="AT23" s="9"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AO24" s="9"/>
-      <c r="AR24" s="9"/>
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AQ24" s="9"/>
+      <c r="AT24" s="9"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AO25" s="9"/>
-      <c r="AR25" s="9"/>
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AQ25" s="9"/>
+      <c r="AT25" s="9"/>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AO26" s="9"/>
-      <c r="AR26" s="9"/>
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AQ26" s="9"/>
+      <c r="AT26" s="9"/>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AO27" s="9"/>
-      <c r="AR27" s="9"/>
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AQ27" s="9"/>
+      <c r="AT27" s="9"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AO28" s="9"/>
-      <c r="AR28" s="9"/>
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AQ28" s="9"/>
+      <c r="AT28" s="9"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="AO29" s="9"/>
-      <c r="AR29" s="9"/>
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AQ29" s="9"/>
+      <c r="AT29" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>